<commit_message>
changes as of 06/12
</commit_message>
<xml_diff>
--- a/excel_files/example_analysis.xlsx
+++ b/excel_files/example_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adnan\Documents\GitHub\Killa-Design-Structures-code\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adnan.a\Documents\GitHub\Killa-Design-Structures-code\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC703E3-65CB-43A1-BAA9-406667B44E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8720A064-C2FE-4836-8E20-0F6E2428A4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{67CE0F2D-70B1-417C-92DF-201EBF35E29E}"/>
+    <workbookView xWindow="38280" yWindow="1620" windowWidth="30960" windowHeight="16920" xr2:uid="{67CE0F2D-70B1-417C-92DF-201EBF35E29E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -823,11 +823,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17079B29-2E32-4F67-BA28-C814F6E3F5EC}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N102" sqref="N102"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -4374,11 +4377,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF6D285E-6404-4EAE-97A4-20A4BA5E2026}">
   <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="S107" sqref="S107"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
end of day changes
</commit_message>
<xml_diff>
--- a/excel_files/example_analysis.xlsx
+++ b/excel_files/example_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adnan.a\Documents\GitHub\Killa-Design-Structures-code\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB6CF30-F9D5-429A-AD6C-40EFE2839481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E739EA7-57FC-4A60-808E-13E1F2B2F79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1620" windowWidth="30960" windowHeight="16920" activeTab="1" xr2:uid="{67CE0F2D-70B1-417C-92DF-201EBF35E29E}"/>
   </bookViews>
@@ -824,7 +824,7 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="A16" sqref="A16:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4378,7 +4378,7 @@
   <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>